<commit_message>
base region list added.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/StandardPIOT_RootClassification.xlsx
+++ b/ConcordanceLibrary/StandardPIOT_RootClassification.xlsx
@@ -20,7 +20,7 @@
     <sheet name="BACIRegions" sheetId="6" r:id="rId6"/>
     <sheet name="BaseProducts" sheetId="7" r:id="rId7"/>
     <sheet name="BaseIndustries" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
+    <sheet name="BaseRegions" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4213" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4159" uniqueCount="1344">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -4057,19 +4057,13 @@
     <t>BaseIndustryCode</t>
   </si>
   <si>
-    <t>Industries</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>Boundary Input</t>
-  </si>
-  <si>
-    <t>Inputs from Nature</t>
-  </si>
-  <si>
-    <t>EoL Scrap</t>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>BaseRegionCode</t>
+  </si>
+  <si>
+    <t>BaseRegionName</t>
   </si>
 </sst>
 </file>
@@ -4137,7 +4131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4169,15 +4163,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -26004,9 +25989,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -26210,7 +26193,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26394,733 +26377,305 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:AS47"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="2.81640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="18" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>1341</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>8</v>
-      </c>
-      <c r="L2">
-        <v>9</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>11</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2">
-        <v>13</v>
-      </c>
-      <c r="Q2">
-        <v>14</v>
-      </c>
-      <c r="R2">
-        <v>15</v>
-      </c>
-      <c r="S2">
-        <v>16</v>
-      </c>
-      <c r="T2">
-        <v>17</v>
-      </c>
-      <c r="U2">
-        <v>18</v>
-      </c>
-      <c r="V2">
-        <v>19</v>
-      </c>
-      <c r="W2">
-        <v>20</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>2</v>
-      </c>
-      <c r="Z2">
-        <v>3</v>
-      </c>
-      <c r="AA2">
-        <v>4</v>
-      </c>
-      <c r="AB2">
-        <v>5</v>
-      </c>
-      <c r="AC2">
-        <v>6</v>
-      </c>
-      <c r="AD2">
-        <v>7</v>
-      </c>
-      <c r="AE2">
-        <v>8</v>
-      </c>
-      <c r="AF2">
-        <v>9</v>
-      </c>
-      <c r="AG2">
-        <v>10</v>
-      </c>
-      <c r="AH2">
-        <v>11</v>
-      </c>
-      <c r="AI2">
-        <v>12</v>
-      </c>
-      <c r="AJ2">
-        <v>13</v>
-      </c>
-      <c r="AK2">
-        <v>14</v>
-      </c>
-      <c r="AL2">
-        <v>15</v>
-      </c>
-      <c r="AM2">
-        <v>16</v>
-      </c>
-      <c r="AN2">
-        <v>17</v>
-      </c>
-      <c r="AO2">
-        <v>18</v>
-      </c>
-      <c r="AP2">
-        <v>19</v>
-      </c>
-      <c r="AQ2">
-        <v>20</v>
-      </c>
-      <c r="AR2">
-        <v>21</v>
-      </c>
-      <c r="AS2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="D3" t="s">
-        <v>256</v>
-      </c>
-      <c r="E3" t="s">
-        <v>252</v>
-      </c>
-      <c r="F3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1335</v>
-      </c>
-      <c r="H3" t="s">
-        <v>254</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1336</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1337</v>
-      </c>
-      <c r="K3" t="s">
-        <v>552</v>
-      </c>
-      <c r="L3" t="s">
-        <v>563</v>
-      </c>
-      <c r="M3" t="s">
-        <v>255</v>
-      </c>
-      <c r="N3" t="s">
-        <v>583</v>
-      </c>
-      <c r="O3" t="s">
-        <v>584</v>
-      </c>
-      <c r="P3" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>586</v>
-      </c>
-      <c r="R3" t="s">
-        <v>587</v>
-      </c>
-      <c r="S3" t="s">
-        <v>588</v>
-      </c>
-      <c r="T3" t="s">
-        <v>589</v>
-      </c>
-      <c r="U3" t="s">
-        <v>590</v>
-      </c>
-      <c r="V3" t="s">
-        <v>591</v>
-      </c>
-      <c r="W3" t="s">
-        <v>1338</v>
-      </c>
-      <c r="X3" t="s">
-        <v>279</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>271</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>272</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>310</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>1328</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>1329</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>1330</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>214</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>1331</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>216</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>221</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>222</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>224</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
-      <c r="B16">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
-      <c r="B20">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="17"/>
-      <c r="B23">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
-        <v>1342</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="17"/>
-      <c r="B30">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="17"/>
-      <c r="B31">
-        <v>8</v>
-      </c>
-      <c r="C31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="17"/>
-      <c r="B32">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="17"/>
-      <c r="B33">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="17"/>
-      <c r="B34">
-        <v>11</v>
-      </c>
-      <c r="C34" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="17"/>
-      <c r="B35">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="17"/>
-      <c r="B36">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="17"/>
-      <c r="B37">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="17"/>
-      <c r="B38">
-        <v>15</v>
-      </c>
-      <c r="C38" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="17"/>
-      <c r="B39">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="17"/>
-      <c r="B40">
-        <v>17</v>
-      </c>
-      <c r="C40" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="17"/>
-      <c r="B41">
-        <v>18</v>
-      </c>
-      <c r="C41" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="17"/>
-      <c r="B42">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="17"/>
-      <c r="B43">
-        <v>20</v>
-      </c>
-      <c r="C43" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="17"/>
-      <c r="B44">
-        <v>21</v>
-      </c>
-      <c r="C44" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="17"/>
-      <c r="B45">
-        <v>22</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="16" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="16"/>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1345</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A4:A23"/>
-    <mergeCell ref="A24:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="D1:W1"/>
-    <mergeCell ref="X1:AS1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>